<commit_message>
5 test cases for the Library Card Entry updated.
</commit_message>
<xml_diff>
--- a/src/test/resources/LibraryCardData.xlsx
+++ b/src/test/resources/LibraryCardData.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{707C9C49-78A3-4034-8608-1BF0C83A0376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91920\git\Sprint-Project\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB05D202-594C-4F3C-B067-E9082ABD8F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{837E9CB1-9313-4AF9-A6CD-FD0C2C40EB1B}"/>
   </bookViews>
@@ -11,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="36">
   <si>
     <t>first</t>
   </si>
@@ -65,9 +69,6 @@
     <t>cognizant</t>
   </si>
   <si>
-    <t>Apply</t>
-  </si>
-  <si>
     <t>Valid</t>
   </si>
   <si>
@@ -78,13 +79,67 @@
   </si>
   <si>
     <t>G.L bAJAJS</t>
+  </si>
+  <si>
+    <t>Somuik</t>
+  </si>
+  <si>
+    <t>Pal</t>
+  </si>
+  <si>
+    <t>Soumik123@gmail.com</t>
+  </si>
+  <si>
+    <t>Apply New Card</t>
+  </si>
+  <si>
+    <t>Renewal Old Card</t>
+  </si>
+  <si>
+    <t>IIT</t>
+  </si>
+  <si>
+    <t>Abhinav</t>
+  </si>
+  <si>
+    <t>Pandey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jayantika </t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>jayantika@gmail.com</t>
+  </si>
+  <si>
+    <t>abhinav@gmail.com</t>
+  </si>
+  <si>
+    <t>123@gmail.com</t>
+  </si>
+  <si>
+    <t>##123#gmail.com</t>
+  </si>
+  <si>
+    <t>.com</t>
+  </si>
+  <si>
+    <t>jayantika@gmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                            Abcdefgh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           abc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,16 +155,58 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3300"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -117,21 +214,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -440,14 +570,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85AF274-DC10-48DD-B582-522A03D07E52}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
     <col min="4" max="4" width="17.6328125" customWidth="1"/>
     <col min="5" max="5" width="21.26953125" customWidth="1"/>
     <col min="6" max="7" width="16.453125" customWidth="1"/>
@@ -456,148 +588,467 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
-        <v>24</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="2">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>9205106245</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2">
+        <v>9205106245</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2">
+        <v>9205106245</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9205106245</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="7">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="7">
+        <v>9205106245</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="7">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="7">
+        <v>9205106245</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="7">
+        <v>24</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="7">
+        <v>9205106245</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="8">
+        <v>24</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="8">
+        <v>9205106245</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C10" s="8">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3">
+      <c r="E10" s="8">
         <v>9205106245</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="H10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="8">
+        <v>-24</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="8">
+        <v>9205106245</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="8">
+        <v>9205106245</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
-        <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C13" s="4">
+        <v>24</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E4">
-        <v>9205106245</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="4">
+        <v>24</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="4">
+        <v>9.2023009293232898E+19</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4">
+        <v>24</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="4">
+        <v>-9205106245</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="H16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>9205106245</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -606,6 +1057,17 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{18954968-D85C-477A-9D66-7FD78AA3708E}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{581357F6-DAE7-44BA-9004-D9C301293F08}"/>
     <hyperlink ref="D5" r:id="rId4" xr:uid="{F095F4A7-E76B-4F00-96CB-3A2A35D364BB}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{C73282AC-5D74-4FE9-8D61-B64A44AFF8E7}"/>
+    <hyperlink ref="D7" r:id="rId6" display="Soumik123@gmail.com" xr:uid="{327645FB-EC77-48CC-9257-F1D4BC796D9A}"/>
+    <hyperlink ref="D8" r:id="rId7" display="abhinav@gmail.com" xr:uid="{DE327765-1D4B-4A0F-8913-2FCB889ACAD6}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{DBAD6DAD-7F7D-4130-91BD-026BD2D55BCB}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{69E2C59D-7258-4CB5-A29C-9A7136FDA3DA}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{1F77C067-1C9E-4C5F-90D0-C53286265015}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{3BA8ED16-0658-4C9B-AF7F-743046B57F4E}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{0C54F4A6-5234-49B1-9C8F-9F444C131CC6}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{8E570F40-F82A-4083-A73A-1BB42128E28B}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{6FF77E50-884B-4571-B444-DEC3CAA46AB1}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{6573257C-5C93-416E-9F2B-03174C22AB3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
JavaExceuter added to scroll to the result
</commit_message>
<xml_diff>
--- a/src/test/resources/LibraryCardData.xlsx
+++ b/src/test/resources/LibraryCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91920\git\Sprint-Project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB05D202-594C-4F3C-B067-E9082ABD8F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417B548C-34A0-4617-A0A1-24342250D29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{837E9CB1-9313-4AF9-A6CD-FD0C2C40EB1B}"/>
   </bookViews>
@@ -573,7 +573,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -827,7 +827,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="8">
-        <v>24</v>
+        <v>10000</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>33</v>

</xml_diff>